<commit_message>
Upload Updated Test Matrix
</commit_message>
<xml_diff>
--- a/document/V2_Test_Matrix.xlsx
+++ b/document/V2_Test_Matrix.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sprint 1 - Testing" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sprint 2 &amp; 3 - Testing" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -115,6 +116,100 @@
   </si>
   <si>
     <t>Tester: Reanne Rylle C. Jalipa</t>
+  </si>
+  <si>
+    <t>TC2_01</t>
+  </si>
+  <si>
+    <t>(Automated) Verify user can sign up</t>
+  </si>
+  <si>
+    <t>Application is opened</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to sign-up component
+2. Enter required data
+3. Submit </t>
+  </si>
+  <si>
+    <t>Automated input of data will partially finish creating the account</t>
+  </si>
+  <si>
+    <t>User is partially signed up, email confirmation is required</t>
+  </si>
+  <si>
+    <t>TC2_02</t>
+  </si>
+  <si>
+    <t>(Automated) Registered user can log in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to sign-in component
+2. Enter valid credentials
+3. Submit </t>
+  </si>
+  <si>
+    <t>User is successfully logged in (automated)</t>
+  </si>
+  <si>
+    <t>TC2_03</t>
+  </si>
+  <si>
+    <t>Verify that sign-in data is in the database</t>
+  </si>
+  <si>
+    <t>User has signed in already</t>
+  </si>
+  <si>
+    <t>1. Check if data is stored in the database</t>
+  </si>
+  <si>
+    <t>the created sign-in data is stored in database</t>
+  </si>
+  <si>
+    <t>the created sign-in data appeared on the database and is functional</t>
+  </si>
+  <si>
+    <t>TC2_04</t>
+  </si>
+  <si>
+    <t>Ensure Email authentication is functional</t>
+  </si>
+  <si>
+    <t>User must fill up the sign-up form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User must fill up sign-in form
+2. User must submit the form
+3. User will recieve a confirmation link through the submitted email
+</t>
+  </si>
+  <si>
+    <t>Upon clicking the link, the email will verify the email and allow the user to log in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authentication link is working and user can use the email to log in </t>
+  </si>
+  <si>
+    <t>Add alerts/notifications for visual confirmation to users</t>
+  </si>
+  <si>
+    <t>TC2_05</t>
+  </si>
+  <si>
+    <t>Test Forgot Password functionality</t>
+  </si>
+  <si>
+    <t>User must click "Forgot Password"</t>
+  </si>
+  <si>
+    <t>1. Click forgot Password</t>
+  </si>
+  <si>
+    <t>On click, the user is redirected to forgot password and is able to change it</t>
+  </si>
+  <si>
+    <t>User is redirected and is able to change password upon navigating to "forgot password"</t>
   </si>
 </sst>
 </file>
@@ -174,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -190,6 +285,12 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -199,6 +300,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -540,7 +645,7 @@
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5">
+    <row r="5" ht="55.5" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1573,4 +1678,242 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="35.57"/>
+    <col customWidth="1" min="4" max="4" width="22.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>